<commit_message>
modify index of rolelevel
</commit_message>
<xml_diff>
--- a/rolelevel.xlsx
+++ b/rolelevel.xlsx
@@ -18,10 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>level</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>exp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -39,6 +35,10 @@
   </si>
   <si>
     <t>maxtravellernum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -386,7 +386,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -398,22 +398,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -421,7 +421,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f>10+2*(INDEX(A2:A2,1,1)-1)+(INDEX(A2:A2,1,1)+1)*(INDEX(A2:A2,1,1)+2)*10</f>
+        <f t="shared" ref="B2:B21" si="0">10+2*(INDEX(A2:A2,1,1)-1)+(INDEX(A2:A2,1,1)+1)*(INDEX(A2:A2,1,1)+2)*10</f>
         <v>70</v>
       </c>
       <c r="C2">
@@ -442,7 +442,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f>10+2*(INDEX(A3:A3,1,1)-1)+(INDEX(A3:A3,1,1)+1)*(INDEX(A3:A3,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="C3">
@@ -463,7 +463,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <f>10+2*(INDEX(A4:A4,1,1)-1)+(INDEX(A4:A4,1,1)+1)*(INDEX(A4:A4,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>214</v>
       </c>
       <c r="C4">
@@ -484,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f>10+2*(INDEX(A5:A5,1,1)-1)+(INDEX(A5:A5,1,1)+1)*(INDEX(A5:A5,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>316</v>
       </c>
       <c r="C5">
@@ -505,7 +505,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <f>10+2*(INDEX(A6:A6,1,1)-1)+(INDEX(A6:A6,1,1)+1)*(INDEX(A6:A6,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>438</v>
       </c>
       <c r="C6">
@@ -526,7 +526,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <f>10+2*(INDEX(A7:A7,1,1)-1)+(INDEX(A7:A7,1,1)+1)*(INDEX(A7:A7,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>580</v>
       </c>
       <c r="C7">
@@ -547,7 +547,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <f>10+2*(INDEX(A8:A8,1,1)-1)+(INDEX(A8:A8,1,1)+1)*(INDEX(A8:A8,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>742</v>
       </c>
       <c r="C8">
@@ -568,7 +568,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <f>10+2*(INDEX(A9:A9,1,1)-1)+(INDEX(A9:A9,1,1)+1)*(INDEX(A9:A9,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>924</v>
       </c>
       <c r="C9">
@@ -589,7 +589,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <f>10+2*(INDEX(A10:A10,1,1)-1)+(INDEX(A10:A10,1,1)+1)*(INDEX(A10:A10,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>1126</v>
       </c>
       <c r="C10">
@@ -610,7 +610,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <f>10+2*(INDEX(A11:A11,1,1)-1)+(INDEX(A11:A11,1,1)+1)*(INDEX(A11:A11,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>1348</v>
       </c>
       <c r="C11">
@@ -631,7 +631,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <f>10+2*(INDEX(A12:A12,1,1)-1)+(INDEX(A12:A12,1,1)+1)*(INDEX(A12:A12,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>1590</v>
       </c>
       <c r="C12">
@@ -652,7 +652,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <f>10+2*(INDEX(A13:A13,1,1)-1)+(INDEX(A13:A13,1,1)+1)*(INDEX(A13:A13,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>1852</v>
       </c>
       <c r="C13">
@@ -673,7 +673,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <f>10+2*(INDEX(A14:A14,1,1)-1)+(INDEX(A14:A14,1,1)+1)*(INDEX(A14:A14,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>2134</v>
       </c>
       <c r="C14">
@@ -694,7 +694,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <f>10+2*(INDEX(A15:A15,1,1)-1)+(INDEX(A15:A15,1,1)+1)*(INDEX(A15:A15,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>2436</v>
       </c>
       <c r="C15">
@@ -715,7 +715,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <f>10+2*(INDEX(A16:A16,1,1)-1)+(INDEX(A16:A16,1,1)+1)*(INDEX(A16:A16,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>2758</v>
       </c>
       <c r="C16">
@@ -736,7 +736,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <f>10+2*(INDEX(A17:A17,1,1)-1)+(INDEX(A17:A17,1,1)+1)*(INDEX(A17:A17,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>3100</v>
       </c>
       <c r="C17">
@@ -757,7 +757,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <f>10+2*(INDEX(A18:A18,1,1)-1)+(INDEX(A18:A18,1,1)+1)*(INDEX(A18:A18,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>3462</v>
       </c>
       <c r="C18">
@@ -778,7 +778,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <f>10+2*(INDEX(A19:A19,1,1)-1)+(INDEX(A19:A19,1,1)+1)*(INDEX(A19:A19,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>3844</v>
       </c>
       <c r="C19">
@@ -799,7 +799,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <f>10+2*(INDEX(A20:A20,1,1)-1)+(INDEX(A20:A20,1,1)+1)*(INDEX(A20:A20,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>4246</v>
       </c>
       <c r="C20">
@@ -820,7 +820,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <f>10+2*(INDEX(A21:A21,1,1)-1)+(INDEX(A21:A21,1,1)+1)*(INDEX(A21:A21,1,1)+2)*10</f>
+        <f t="shared" si="0"/>
         <v>4668</v>
       </c>
       <c r="C21">

</xml_diff>